<commit_message>
Add README.md file and update BackPropagationSheet.xlsx
</commit_message>
<xml_diff>
--- a/Part 1/BackPropagationSheet.xlsx
+++ b/Part 1/BackPropagationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aakashvardhan/Library/CloudStorage/GoogleDrive-vardhan.aakash1@gmail.com/My Drive/ERA v2/Session 6/Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D460ED7D-CB73-684D-BB2A-2338E95CA834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A143863-8335-E14F-BC98-70043949B8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-3100" windowWidth="51200" windowHeight="21100" tabRatio="411" activeTab="5" xr2:uid="{9439E314-D218-4DC1-801D-FD5CAA68FFFB}"/>
+    <workbookView xWindow="33600" yWindow="-3100" windowWidth="51200" windowHeight="21100" tabRatio="411" activeTab="3" xr2:uid="{9439E314-D218-4DC1-801D-FD5CAA68FFFB}"/>
   </bookViews>
   <sheets>
     <sheet name="LR = 0.1" sheetId="3" r:id="rId1"/>
@@ -421,6 +421,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -430,6 +439,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -437,24 +455,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -26393,7 +26393,7 @@
   <dimension ref="A31:AE100"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:AE34"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -34828,8 +34828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60F31F9-45DE-EB43-B791-A856C5F866C6}">
   <dimension ref="A31:AE100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -43295,101 +43295,101 @@
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="14" t="s">
+      <c r="K5" s="21"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="16"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22"/>
     </row>
     <row r="6" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="11" t="s">
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="13"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="16"/>
     </row>
     <row r="7" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="11" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="13"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="16"/>
     </row>
     <row r="8" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="11" t="s">
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="13"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="16"/>
     </row>
     <row r="9" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="11" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="13"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="20" t="s">
+      <c r="K10" s="15"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="22"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
     </row>
     <row r="11" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="2">
         <v>3</v>
       </c>
@@ -43400,246 +43400,246 @@
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="11" t="s">
+      <c r="K12" s="15"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="12"/>
-      <c r="R12" s="13"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="16"/>
     </row>
     <row r="13" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="11" t="s">
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="12"/>
-      <c r="R13" s="13"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="16"/>
     </row>
     <row r="14" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="11" t="s">
+      <c r="K14" s="15"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
-      <c r="R14" s="13"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="16"/>
     </row>
     <row r="15" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="11" t="s">
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="13"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="16"/>
     </row>
     <row r="16" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J16" s="17">
+      <c r="J16" s="11">
         <v>4</v>
       </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="19"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="13"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C17" s="17">
+      <c r="C17" s="11">
         <v>5</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
-      <c r="J17" s="11" t="s">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
+      <c r="J17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="13"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="16"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-      <c r="J18" s="11" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="16"/>
+      <c r="J18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="13"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="16"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="13"/>
-      <c r="J19" s="11" t="s">
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="J19" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="13"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="16"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="22"/>
-      <c r="J20" s="20" t="s">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="J20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="22"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C22" s="17">
+      <c r="C22" s="11">
         <v>6</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="19"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="13"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="13"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="13"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="13"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="22"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="19"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
@@ -52034,11 +52034,28 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C22:O22"/>
-    <mergeCell ref="C23:O23"/>
-    <mergeCell ref="C24:O24"/>
-    <mergeCell ref="C25:O25"/>
-    <mergeCell ref="C26:O26"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="M7:R7"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="J16:R16"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="M12:R12"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="M14:R14"/>
+    <mergeCell ref="M15:R15"/>
     <mergeCell ref="J17:R17"/>
     <mergeCell ref="J18:R18"/>
     <mergeCell ref="J19:R19"/>
@@ -52047,28 +52064,11 @@
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
-    <mergeCell ref="M10:R10"/>
-    <mergeCell ref="M12:R12"/>
-    <mergeCell ref="M13:R13"/>
-    <mergeCell ref="M14:R14"/>
-    <mergeCell ref="M15:R15"/>
-    <mergeCell ref="J16:R16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="M7:R7"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="C22:O22"/>
+    <mergeCell ref="C23:O23"/>
+    <mergeCell ref="C24:O24"/>
+    <mergeCell ref="C25:O25"/>
+    <mergeCell ref="C26:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -52083,7 +52083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92CF14C-AE7D-7E48-B947-AC230330DB37}">
   <dimension ref="A31:AE100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update backpropagation tutorial and add simple neural network diagram
</commit_message>
<xml_diff>
--- a/Part 1/BackPropagationSheet.xlsx
+++ b/Part 1/BackPropagationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aakashvardhan/Library/CloudStorage/GoogleDrive-vardhan.aakash1@gmail.com/My Drive/ERA v2/Session 6/Part 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A143863-8335-E14F-BC98-70043949B8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411257FE-4985-E547-A9F2-A995A40AD34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-3100" windowWidth="51200" windowHeight="21100" tabRatio="411" activeTab="3" xr2:uid="{9439E314-D218-4DC1-801D-FD5CAA68FFFB}"/>
+    <workbookView xWindow="36140" yWindow="-2760" windowWidth="51200" windowHeight="21100" tabRatio="411" activeTab="3" xr2:uid="{9439E314-D218-4DC1-801D-FD5CAA68FFFB}"/>
   </bookViews>
   <sheets>
     <sheet name="LR = 0.1" sheetId="3" r:id="rId1"/>
@@ -421,6 +421,24 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -430,15 +448,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -446,15 +455,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -34828,7 +34828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60F31F9-45DE-EB43-B791-A856C5F866C6}">
   <dimension ref="A31:AE100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -43295,101 +43295,101 @@
       <c r="R4" s="5"/>
     </row>
     <row r="5" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="20" t="s">
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="22"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="14" t="s">
+      <c r="K6" s="12"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="16"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="13"/>
     </row>
     <row r="7" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="14" t="s">
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="16"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="13"/>
     </row>
     <row r="8" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="14" t="s">
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="16"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="13"/>
     </row>
     <row r="9" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="14" t="s">
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="16"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="13"/>
     </row>
     <row r="10" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="17" t="s">
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="19"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="22"/>
     </row>
     <row r="11" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="15"/>
-      <c r="L11" s="16"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="13"/>
       <c r="M11" s="2">
         <v>3</v>
       </c>
@@ -43400,246 +43400,246 @@
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="14" t="s">
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="16"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="13"/>
     </row>
     <row r="13" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="14" t="s">
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="16"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="13"/>
     </row>
     <row r="14" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="14" t="s">
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="13"/>
     </row>
     <row r="15" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="15"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="14" t="s">
+      <c r="K15" s="12"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="16"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="13"/>
     </row>
     <row r="16" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J16" s="11">
+      <c r="J16" s="17">
         <v>4</v>
       </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="13"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="19"/>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C17" s="11">
+      <c r="C17" s="17">
         <v>5</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
-      <c r="J17" s="14" t="s">
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="J17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="16"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
-      <c r="J18" s="14" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="J18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="16"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="16"/>
-      <c r="J19" s="14" t="s">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="J19" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="16"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="13"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="J20" s="17" t="s">
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="22"/>
+      <c r="J20" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="19"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="22"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C22" s="11">
+      <c r="C22" s="17">
         <v>6</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="19"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="16"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="13"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="16"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="13"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="16"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="13"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="22"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
@@ -52034,28 +52034,11 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M5:R5"/>
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="M7:R7"/>
-    <mergeCell ref="M8:R8"/>
-    <mergeCell ref="M9:R9"/>
-    <mergeCell ref="J16:R16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M10:R10"/>
-    <mergeCell ref="M12:R12"/>
-    <mergeCell ref="M13:R13"/>
-    <mergeCell ref="M14:R14"/>
-    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="C22:O22"/>
+    <mergeCell ref="C23:O23"/>
+    <mergeCell ref="C24:O24"/>
+    <mergeCell ref="C25:O25"/>
+    <mergeCell ref="C26:O26"/>
     <mergeCell ref="J17:R17"/>
     <mergeCell ref="J18:R18"/>
     <mergeCell ref="J19:R19"/>
@@ -52064,11 +52047,28 @@
     <mergeCell ref="C18:H18"/>
     <mergeCell ref="C19:H19"/>
     <mergeCell ref="C20:H20"/>
-    <mergeCell ref="C22:O22"/>
-    <mergeCell ref="C23:O23"/>
-    <mergeCell ref="C24:O24"/>
-    <mergeCell ref="C25:O25"/>
-    <mergeCell ref="C26:O26"/>
+    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="M12:R12"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="M14:R14"/>
+    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="J16:R16"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M5:R5"/>
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="M7:R7"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>